<commit_message>
Typo in IR2&3 equation
</commit_message>
<xml_diff>
--- a/Sensor.xlsx
+++ b/Sensor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limzui\Documents\GitHub\CE3004-MDP-ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925459B3-3023-40D0-B632-05AE2B121463}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014F522F-97E8-43CC-B760-82F2666A7085}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
+    <workbookView xWindow="768" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="6" r:id="rId1"/>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE365FD-844F-40B5-B0D1-185FCF6C986C}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC94E3C-D284-4D19-92AB-A16814BB168E}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:F28"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated some raw values
</commit_message>
<xml_diff>
--- a/Sensor.xlsx
+++ b/Sensor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brabalawuka\src\CE3004-MDP-ARDUINO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Documents\GitHub\CE3004-MDP-ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016D958A-8ADE-4BA0-92E8-B6DBAB885465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B200030-3114-4B8F-BB2E-AD495CC870A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10560" yWindow="313" windowWidth="19200" windowHeight="10520" activeTab="2" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="6" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -425,16 +423,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE365FD-844F-40B5-B0D1-185FCF6C986C}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -442,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -476,13 +474,13 @@
         <v>630</v>
       </c>
       <c r="E3" s="1">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="F3" s="1">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -496,15 +494,15 @@
         <v>611</v>
       </c>
       <c r="E4" s="1">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="F4" s="1">
-        <v>458</v>
+        <v>477</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -518,15 +516,15 @@
         <v>558</v>
       </c>
       <c r="E5" s="1">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F5" s="1">
-        <v>421</v>
+        <v>437</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -540,15 +538,15 @@
         <v>513</v>
       </c>
       <c r="E6" s="1">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="F6" s="1">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -562,15 +560,15 @@
         <v>471</v>
       </c>
       <c r="E7" s="1">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F7" s="1">
-        <v>363</v>
+        <v>378</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -579,11 +577,11 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>2</v>
       </c>
@@ -591,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0</v>
       </c>
@@ -623,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -641,19 +639,19 @@
       </c>
       <c r="E14">
         <f>1/($E3+E$12)</f>
-        <v>1.8726591760299626E-3</v>
+        <v>1.8867924528301887E-3</v>
       </c>
       <c r="F14">
         <f>1/($F3+F$12)</f>
-        <v>2.004008016032064E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+        <v>1.9305019305019305E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:B19" si="0">1/($B4+B$12)</f>
+        <f t="shared" ref="B15:B18" si="0">1/($B4+B$12)</f>
         <v>1.6025641025641025E-3</v>
       </c>
       <c r="C15">
@@ -666,11 +664,11 @@
       </c>
       <c r="E15">
         <f t="shared" ref="E15:E18" si="3">1/($E4+E$12)</f>
-        <v>2.0366598778004071E-3</v>
+        <v>2.0618556701030928E-3</v>
       </c>
       <c r="F15">
         <f t="shared" ref="F15:F18" si="4">1/($F4+F$12)</f>
-        <v>2.1834061135371178E-3</v>
+        <v>2.0964360587002098E-3</v>
       </c>
       <c r="I15">
         <v>4</v>
@@ -689,14 +687,14 @@
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>3.9585647161544575</v>
+        <v>4.0152826469771803</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
-        <v>4.0030451290792204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+        <v>3.9956796242903643</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -714,11 +712,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>2.2471910112359553E-3</v>
+        <v>2.242152466367713E-3</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>2.3752969121140144E-3</v>
+        <v>2.2883295194508009E-3</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -737,14 +735,14 @@
       </c>
       <c r="M16">
         <f t="shared" si="5"/>
-        <v>5.0971207667915603</v>
+        <v>4.9707213893822111</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
-        <v>4.9939643862839613</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
+        <v>5.0087557528437276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -762,11 +760,11 @@
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>2.403846153846154E-3</v>
+        <v>2.4390243902439024E-3</v>
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
-        <v>2.5706940874035988E-3</v>
+        <v>2.4752475247524753E-3</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -785,14 +783,14 @@
       </c>
       <c r="M17">
         <f t="shared" si="5"/>
-        <v>5.9443145170539822</v>
+        <v>6.013995963640614</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
-        <v>6.0029904846368183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
+        <v>5.9955646228659099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -810,11 +808,11 @@
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>2.6109660574412533E-3</v>
+        <v>2.5974025974025974E-3</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>2.7548209366391185E-3</v>
+        <v>2.6455026455026454E-3</v>
       </c>
       <c r="I18">
         <v>7</v>
@@ -833,14 +831,14 @@
       </c>
       <c r="M18">
         <f t="shared" si="5"/>
-        <v>7.064422577070518</v>
+        <v>6.8532825078672506</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>6.953816902729999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
+        <v>6.894403999264183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I19">
         <v>8</v>
       </c>
@@ -858,14 +856,14 @@
       </c>
       <c r="M19">
         <f t="shared" si="5"/>
-        <v>-0.14172882926401612</v>
+        <v>-0.14469650796900177</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>-0.13751357888148585</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
+        <v>-0.14139917435128274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -873,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -890,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -908,14 +906,14 @@
       </c>
       <c r="E25">
         <f t="shared" si="6"/>
-        <v>-7.0557275128349097</v>
+        <v>-6.9110168174495907</v>
       </c>
       <c r="F25">
         <f t="shared" si="6"/>
-        <v>-7.2720091218179697</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.5">
+        <v>-7.0721770801551234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -933,28 +931,22 @@
       </c>
       <c r="E26">
         <f>SLOPE($A15:$A17,E15:E17)</f>
-        <v>5408.0174844337789</v>
+        <v>5299.2552402469837</v>
       </c>
       <c r="F26">
         <f t="shared" si="7"/>
-        <v>5163.9748469109127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.5">
+        <v>5279.3676480204977</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
-      <c r="D27">
-        <v>8.7535014005602296E-5</v>
-      </c>
-      <c r="F27">
-        <v>2.3895532551367711E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.5">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2</v>
       </c>
@@ -962,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -982,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A4</f>
         <v>4</v>
@@ -1001,14 +993,14 @@
       </c>
       <c r="E36">
         <f t="shared" si="8"/>
-        <v>3.9585647161544575</v>
+        <v>4.0152826469771803</v>
       </c>
       <c r="F36">
         <f t="shared" si="8"/>
-        <v>4.0030451290792204</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+        <v>3.9956796242903643</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A5</f>
         <v>5</v>
@@ -1027,14 +1019,14 @@
       </c>
       <c r="E37">
         <f t="shared" si="9"/>
-        <v>5.0971207667915603</v>
+        <v>4.9707213893822111</v>
       </c>
       <c r="F37">
         <f t="shared" si="9"/>
-        <v>4.9939643862839613</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+        <v>5.0087557528437276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>A6</f>
         <v>6</v>
@@ -1053,14 +1045,14 @@
       </c>
       <c r="E38">
         <f t="shared" si="10"/>
-        <v>5.9443145170539822</v>
+        <v>6.013995963640614</v>
       </c>
       <c r="F38">
         <f t="shared" si="10"/>
-        <v>6.0029904846368183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+        <v>5.9955646228659099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>A7</f>
         <v>7</v>
@@ -1079,24 +1071,24 @@
       </c>
       <c r="E39">
         <f t="shared" si="11"/>
-        <v>7.064422577070518</v>
+        <v>6.8532825078672506</v>
       </c>
       <c r="F39">
         <f t="shared" si="11"/>
-        <v>6.953816902729999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+        <v>6.894403999264183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>A8</f>
         <v>0</v>
       </c>
       <c r="B40" t="e">
-        <f t="shared" ref="B37:B40" si="12">B$26/B8+B$25</f>
+        <f t="shared" ref="B40" si="12">B$26/B8+B$25</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="B36:F40" si="13">(1/C$26)/(C8+(C$25/C$26))-C$12</f>
+        <f t="shared" ref="C40:F40" si="13">(1/C$26)/(C8+(C$25/C$26))-C$12</f>
         <v>-0.13405934701514011</v>
       </c>
       <c r="D40">
@@ -1105,11 +1097,11 @@
       </c>
       <c r="E40">
         <f t="shared" si="13"/>
-        <v>-0.14172882926401612</v>
+        <v>-0.14469650796900177</v>
       </c>
       <c r="F40">
         <f t="shared" si="13"/>
-        <v>-0.13751357888148585</v>
+        <v>-0.14139917435128274</v>
       </c>
     </row>
   </sheetData>
@@ -1122,16 +1114,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC94E3C-D284-4D19-92AB-A16814BB168E}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1139,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1179,7 +1171,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1199,7 +1191,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1219,7 +1211,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -1239,7 +1231,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -1259,7 +1251,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -1279,7 +1271,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -1299,7 +1291,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -1322,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1362,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1410,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1458,7 +1450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20</v>
       </c>
@@ -1506,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1554,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>30</v>
       </c>
@@ -1602,7 +1594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>35</v>
       </c>
@@ -1650,7 +1642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J21">
         <v>35</v>
       </c>
@@ -1675,7 +1667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L23">
         <f>ABS(L15-$J15)+ABS(L16-$J16)+ABS(L17-$J17)+ABS(L18-$J18)+ABS(L19-$J19)+ABS(L20-$J20)+ABS(L21-$J21)</f>
         <v>1</v>
@@ -1697,7 +1689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
@@ -1705,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -1722,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1747,7 +1739,7 @@
         <v>-10.970771331654497</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1772,12 +1764,12 @@
         <v>6222.3754020320584</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>2</v>
       </c>
@@ -1785,7 +1777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1805,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ref="A33:A39" si="5">A3</f>
         <v>5</v>
@@ -1831,7 +1823,7 @@
         <v>3.8092177468064499</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="5"/>
         <v>10</v>
@@ -1857,7 +1849,7 @@
         <v>9.9096830375805993</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -1883,7 +1875,7 @@
         <v>15.849812297794031</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="5"/>
         <v>20</v>
@@ -1909,7 +1901,7 @@
         <v>21.26951572550643</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="5"/>
         <v>25</v>
@@ -1935,7 +1927,7 @@
         <v>26.513417837213325</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="5"/>
         <v>30</v>
@@ -1961,7 +1953,7 @@
         <v>29.173586100810397</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="5"/>
         <v>35</v>
@@ -1997,23 +1989,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558F13F8-FE73-45A7-88B3-F428177E8C39}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2032,7 +2024,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2043,7 +2035,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -2054,7 +2046,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -2065,7 +2057,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>35</v>
       </c>
@@ -2076,29 +2068,29 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>45</v>
       </c>
       <c r="B8" s="1">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C8" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
       <c r="B9" s="1">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C9" s="1">
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -2106,7 +2098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2118,7 +2110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2131,11 +2123,11 @@
         <v>5</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H20" si="1">ROUND(B32,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+        <f t="shared" ref="H15" si="1">ROUND(B32,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2144,7 +2136,7 @@
         <v>2.1276595744680851E-3</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G15:G20" si="2">A5</f>
+        <f t="shared" ref="G16:G20" si="2">A5</f>
         <v>15</v>
       </c>
       <c r="H16">
@@ -2152,7 +2144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2166,10 +2158,10 @@
       </c>
       <c r="H17">
         <f>ROUND(B35,0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>35</v>
       </c>
@@ -2183,16 +2175,16 @@
       </c>
       <c r="H18">
         <f>ROUND(B36,0)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>45</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>4.464285714285714E-3</v>
+        <v>4.329004329004329E-3</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
@@ -2200,16 +2192,16 @@
       </c>
       <c r="H19">
         <f>ROUND(B37,0)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>55</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>5.1020408163265302E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
@@ -2217,20 +2209,20 @@
       </c>
       <c r="H20">
         <f>ROUND(B38,0)</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2240,10 +2232,10 @@
       </c>
       <c r="C25">
         <f>INTERCEPT(A16:A20,B16:B20)</f>
-        <v>-13.223631890637058</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+        <v>-14.800848533965095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2253,20 +2245,20 @@
       </c>
       <c r="C26">
         <f>SLOPE(A16:A20,B16:B20)</f>
-        <v>13208.456295698532</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+        <v>13820.124770452703</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2274,7 +2266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A3</f>
         <v>5</v>
@@ -2285,10 +2277,10 @@
       </c>
       <c r="C32">
         <f>C$26/C3+C$25</f>
-        <v>9.3163959177222111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+        <v>8.7829821323364463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -2298,10 +2290,10 @@
       </c>
       <c r="C33">
         <f t="shared" si="3"/>
-        <v>11.697983761624322</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+        <v>11.274858580096609</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>A5</f>
         <v>15</v>
@@ -2312,63 +2304,63 @@
       </c>
       <c r="C34">
         <f t="shared" si="3"/>
-        <v>14.879466610849178</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+        <v>14.603672254232148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>A6</f>
         <v>25</v>
       </c>
       <c r="B35">
-        <f t="shared" si="3"/>
-        <v>32.405433687897627</v>
+        <f>C$26/B6+C$25</f>
+        <v>24.685222238756914</v>
       </c>
       <c r="C35">
-        <f t="shared" si="3"/>
-        <v>24.514814668501607</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+        <f>C$26/C6+C$25</f>
+        <v>24.685222238756914</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A7</f>
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" si="3"/>
-        <v>52.367843923625998</v>
+        <f t="shared" ref="B36:B38" si="4">C$26/B7+C$25</f>
+        <v>36.384798764007883</v>
       </c>
       <c r="C36">
-        <f t="shared" si="3"/>
-        <v>35.6965766119501</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+        <f t="shared" ref="C36:C38" si="5">C$26/C7+C$25</f>
+        <v>36.384798764007883</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A8</f>
         <v>45</v>
       </c>
       <c r="B37">
-        <f t="shared" si="3"/>
-        <v>70.302821869788204</v>
+        <f t="shared" si="4"/>
+        <v>45.026531424704615</v>
       </c>
       <c r="C37">
-        <f t="shared" si="3"/>
-        <v>45.742690858017099</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+        <f t="shared" si="5"/>
+        <v>46.896137048413046</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>A9</f>
         <v>55</v>
       </c>
       <c r="B38">
-        <f t="shared" si="3"/>
-        <v>85.341467973713037</v>
+        <f t="shared" si="4"/>
+        <v>54.299775318298416</v>
       </c>
       <c r="C38">
-        <f t="shared" si="3"/>
-        <v>54.16645125068198</v>
+        <f t="shared" si="5"/>
+        <v>55.709992131609923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes for 19/3 testing
</commit_message>
<xml_diff>
--- a/Sensor.xlsx
+++ b/Sensor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Documents\GitHub\CE3004-MDP-ARDUINO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limzui\Documents\GitHub\CE3004-MDP-ARDUINO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B200030-3114-4B8F-BB2E-AD495CC870A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2173A28-A3D5-4136-B440-EA0D6FE64454}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6602DABA-150B-41F0-8105-E6E9BFF209EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="6" r:id="rId1"/>
@@ -427,12 +427,12 @@
       <selection activeCell="E25" sqref="E25:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -480,7 +480,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -502,7 +502,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -524,7 +524,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -546,7 +546,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -568,7 +568,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -577,11 +577,11 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
         <v>2</v>
       </c>
@@ -589,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -646,7 +646,7 @@
         <v>1.9305019305019305E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -694,7 +694,7 @@
         <v>3.9956796242903643</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -742,7 +742,7 @@
         <v>5.0087557528437276</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -790,7 +790,7 @@
         <v>5.9955646228659099</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7</v>
       </c>
@@ -838,7 +838,7 @@
         <v>6.894403999264183</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I19">
         <v>8</v>
       </c>
@@ -863,7 +863,7 @@
         <v>-0.14139917435128274</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -871,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -888,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -913,7 +913,7 @@
         <v>-7.0721770801551234</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -938,15 +938,15 @@
         <v>5279.3676480204977</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>2</v>
       </c>
@@ -954,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>A4</f>
         <v>4</v>
@@ -1000,7 +1000,7 @@
         <v>3.9956796242903643</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>A5</f>
         <v>5</v>
@@ -1026,7 +1026,7 @@
         <v>5.0087557528437276</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>A6</f>
         <v>6</v>
@@ -1052,7 +1052,7 @@
         <v>5.9955646228659099</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>A7</f>
         <v>7</v>
@@ -1078,7 +1078,7 @@
         <v>6.894403999264183</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>A8</f>
         <v>0</v>
@@ -1114,16 +1114,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC94E3C-D284-4D19-92AB-A16814BB168E}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1165,13 +1165,13 @@
         <v>558</v>
       </c>
       <c r="E3" s="1">
-        <v>445</v>
+        <v>485</v>
       </c>
       <c r="F3" s="1">
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1185,13 +1185,13 @@
         <v>377</v>
       </c>
       <c r="E4" s="1">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="F4" s="1">
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1205,13 +1205,13 @@
         <v>290</v>
       </c>
       <c r="E5" s="1">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="F5" s="1">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -1225,13 +1225,13 @@
         <v>239</v>
       </c>
       <c r="E6" s="1">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="F6" s="1">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -1245,13 +1245,13 @@
         <v>204</v>
       </c>
       <c r="E7" s="1">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F7" s="1">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>30</v>
       </c>
@@ -1265,13 +1265,13 @@
         <v>180</v>
       </c>
       <c r="E8" s="1">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="F8" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>35</v>
       </c>
@@ -1285,13 +1285,13 @@
         <v>170</v>
       </c>
       <c r="E9" s="1">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="F9" s="1">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>2.2471910112359553E-3</v>
+        <v>2.0618556701030928E-3</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -1354,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>3.1545741324921135E-3</v>
+        <v>2.976190476190476E-3</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
@@ -1395,14 +1395,14 @@
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>4.0650406504065045E-3</v>
+        <v>3.8610038610038611E-3</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
@@ -1450,7 +1450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20</v>
       </c>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
+        <v>4.6511627906976744E-3</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
@@ -1491,14 +1491,14 @@
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P17">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>5.7803468208092483E-3</v>
+        <v>5.4054054054054057E-3</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
@@ -1546,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>30</v>
       </c>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>6.6666666666666671E-3</v>
+        <v>6.0606060606060606E-3</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
@@ -1587,14 +1587,14 @@
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P19">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>35</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>7.462686567164179E-3</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
@@ -1642,7 +1642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J21">
         <v>35</v>
       </c>
@@ -1660,14 +1660,14 @@
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P21">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L23">
         <f>ABS(L15-$J15)+ABS(L16-$J16)+ABS(L17-$J17)+ABS(L18-$J18)+ABS(L19-$J19)+ABS(L20-$J20)+ABS(L21-$J21)</f>
         <v>1</v>
@@ -1682,14 +1682,14 @@
       </c>
       <c r="O23">
         <f>ABS(O15-$J15)+ABS(O16-$J16)+ABS(O17-$J17)+ABS(O18-$J18)+ABS(O19-$J19)+ABS(O20-$J20)+ABS(O21-$J21)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P23">
         <f>ABS(P15-$J15)+ABS(P16-$J16)+ABS(P17-$J17)+ABS(P18-$J18)+ABS(P19-$J19)+ABS(P20-$J20)+ABS(P21-$J21)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>2</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1732,14 +1732,14 @@
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>-8.1733882321741866</v>
+        <v>-9.273311963961703</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
         <v>-10.970771331654497</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1757,19 +1757,19 @@
       </c>
       <c r="E27">
         <f t="shared" si="4"/>
-        <v>5736.8750184437049</v>
+        <v>6467.6289861336109</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
         <v>6222.3754020320584</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>2</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" ref="A33:A39" si="5">A3</f>
         <v>5</v>
@@ -1816,14 +1816,14 @@
       </c>
       <c r="E33">
         <f t="shared" si="6"/>
-        <v>4.7184657418566101</v>
+        <v>4.062005533220999</v>
       </c>
       <c r="F33">
         <f t="shared" si="6"/>
         <v>3.8092177468064499</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="5"/>
         <v>10</v>
@@ -1842,14 +1842,14 @@
       </c>
       <c r="E34">
         <f t="shared" si="7"/>
-        <v>9.9240093023485407</v>
+        <v>9.9755838281026143</v>
       </c>
       <c r="F34">
         <f t="shared" si="7"/>
         <v>9.9096830375805993</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -1868,14 +1868,14 @@
       </c>
       <c r="E35">
         <f t="shared" si="7"/>
-        <v>15.147241924101035</v>
+        <v>15.698228523040655</v>
       </c>
       <c r="F35">
         <f t="shared" si="7"/>
         <v>15.849812297794031</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="5"/>
         <v>20</v>
@@ -1894,14 +1894,14 @@
       </c>
       <c r="E36">
         <f t="shared" si="7"/>
-        <v>20.510986860044337</v>
+        <v>20.808683320380673</v>
       </c>
       <c r="F36">
         <f t="shared" si="7"/>
         <v>21.26951572550643</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="5"/>
         <v>25</v>
@@ -1920,14 +1920,14 @@
       </c>
       <c r="E37">
         <f t="shared" si="7"/>
-        <v>24.987739042066881</v>
+        <v>25.686844717841602</v>
       </c>
       <c r="F37">
         <f t="shared" si="7"/>
         <v>26.513417837213325</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="5"/>
         <v>30</v>
@@ -1946,14 +1946,14 @@
       </c>
       <c r="E38">
         <f t="shared" si="7"/>
-        <v>30.072445224117178</v>
+        <v>29.924439467151089</v>
       </c>
       <c r="F38">
         <f t="shared" si="7"/>
         <v>29.173586100810397</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="5"/>
         <v>35</v>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="7"/>
-        <v>34.639111905465398</v>
+        <v>33.84421461026237</v>
       </c>
       <c r="F39">
         <f t="shared" si="7"/>
@@ -1989,23 +1989,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558F13F8-FE73-45A7-88B3-F428177E8C39}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>15</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>25</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>35</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>45</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>55</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>35</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>45</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>55</v>
       </c>
@@ -2212,17 +2212,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>-14.800848533965095</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2248,17 +2248,17 @@
         <v>13820.124770452703</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>A3</f>
         <v>5</v>
@@ -2280,12 +2280,12 @@
         <v>8.7829821323364463</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:C38" si="3">B$26/B4+B$25</f>
+        <f t="shared" ref="B33:C34" si="3">B$26/B4+B$25</f>
         <v>9.5239917667561471</v>
       </c>
       <c r="C33">
@@ -2293,7 +2293,7 @@
         <v>11.274858580096609</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>A5</f>
         <v>15</v>
@@ -2307,7 +2307,7 @@
         <v>14.603672254232148</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>A6</f>
         <v>25</v>
@@ -2321,7 +2321,7 @@
         <v>24.685222238756914</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>A7</f>
         <v>35</v>
@@ -2335,7 +2335,7 @@
         <v>36.384798764007883</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>A8</f>
         <v>45</v>
@@ -2349,7 +2349,7 @@
         <v>46.896137048413046</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>A9</f>
         <v>55</v>

</xml_diff>